<commit_message>
updating manuscript so people can review it!
</commit_message>
<xml_diff>
--- a/code/manuscript/dataset_list.xlsx
+++ b/code/manuscript/dataset_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erinbuchanan/GitHub/Research/2_projects/SPAML/word2manylanguages/code/manuscript/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F16C0F42-2F8E-904B-85BD-BFC94BCEEE65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E293D131-68E2-A64B-9D83-86C11503726D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{C83DC00A-6ADC-5B4F-889C-CB6F261153D3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t>Language</t>
   </si>
@@ -54,16 +54,69 @@
   </si>
   <si>
     <t>50 (1-6), 100 (1-4)</t>
+  </si>
+  <si>
+    <t>Catalan</t>
+  </si>
+  <si>
+    <t>10.5281/zenodo.17352129</t>
+  </si>
+  <si>
+    <t>50 (1-6), 100 (1-6), 200 (1-6), 300 (1-6), 600 (1-6)</t>
+  </si>
+  <si>
+    <t>10.5281/zenodo.17344027</t>
+  </si>
+  <si>
+    <t>Bosnian</t>
+  </si>
+  <si>
+    <t>10.5281/zenodo.17328169</t>
+  </si>
+  <si>
+    <t>Afrikaans</t>
+  </si>
+  <si>
+    <t>Arabic</t>
+  </si>
+  <si>
+    <t>50 (1-6), 100 (1-6), 200 (1-6), 300 (1-4), 300_5_cbow</t>
+  </si>
+  <si>
+    <t>300_5_sg, 300 (6), 500 (1-6)</t>
+  </si>
+  <si>
+    <t>10.5281/zenodo.17334562</t>
+  </si>
+  <si>
+    <t>French</t>
+  </si>
+  <si>
+    <t>10.5281/zenodo.17337550</t>
+  </si>
+  <si>
+    <t>10.5281/zenodo.17343732</t>
+  </si>
+  <si>
+    <t>Galician</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -86,13 +139,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -425,15 +481,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A43873B4-8DCC-7349-8F6E-C461FA9A46F7}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -459,6 +515,83 @@
         <v>2</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>